<commit_message>
add codition state .xlsx file
</commit_message>
<xml_diff>
--- a/code/Buttons Contition States.xlsx
+++ b/code/Buttons Contition States.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TSIMPOS\Documents\lampIR\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4C04986-61FD-4AAB-B776-B006B7DB6718}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6937FEFD-2E4C-4453-B61E-8EAB72E9DBAA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9F8D86CB-A4AA-4D8F-B057-4C611496FE9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
+    <sheet name="EEPROM" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>A</t>
   </si>
@@ -81,7 +82,28 @@
     <t>Output</t>
   </si>
   <si>
-    <t>Cause</t>
+    <t>Index Event</t>
+  </si>
+  <si>
+    <t>Enable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Led on </t>
+  </si>
+  <si>
+    <t>Disable</t>
+  </si>
+  <si>
+    <t>Led off</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>state</t>
   </si>
 </sst>
 </file>
@@ -588,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85E8390D-A126-4B7B-9E1E-48422A8375E2}">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="B4" sqref="B4:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,7 +787,9 @@
       <c r="M5" s="4">
         <v>0</v>
       </c>
-      <c r="N5" s="3"/>
+      <c r="N5" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
@@ -1220,6 +1244,22 @@
         <v>1</v>
       </c>
       <c r="N18" s="7"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1229,4 +1269,78 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F6B317C-4B37-4D4F-9813-3C268A5BF085}">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>